<commit_message>
Update AGENTS figure style guidance
</commit_message>
<xml_diff>
--- a/Symptom_Composition_Pivot_ChartReady.xlsx
+++ b/Symptom_Composition_Pivot_ChartReady.xlsx
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8.880000000000001</v>
+        <v>8.84</v>
       </c>
       <c r="C2" t="n">
         <v>3.13</v>
@@ -495,7 +495,7 @@
         <v>7.11</v>
       </c>
       <c r="E3" t="n">
-        <v>6.28</v>
+        <v>6.27</v>
       </c>
     </row>
     <row r="4">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.68</v>
+        <v>8.77</v>
       </c>
       <c r="C4" t="n">
         <v>5.04</v>
@@ -514,7 +514,7 @@
         <v>7.78</v>
       </c>
       <c r="E4" t="n">
-        <v>6.42</v>
+        <v>6.41</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.31</v>
+        <v>9.140000000000001</v>
       </c>
       <c r="C5" t="n">
         <v>6.91</v>
@@ -533,7 +533,7 @@
         <v>10.13</v>
       </c>
       <c r="E5" t="n">
-        <v>9.619999999999999</v>
+        <v>9.630000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11.69</v>
+        <v>11.71</v>
       </c>
       <c r="C6" t="n">
         <v>6.71</v>
@@ -552,7 +552,7 @@
         <v>14.04</v>
       </c>
       <c r="E6" t="n">
-        <v>14.85</v>
+        <v>14.89</v>
       </c>
     </row>
     <row r="7">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.62</v>
+        <v>1.6</v>
       </c>
       <c r="C7" t="n">
         <v>1.71</v>
@@ -571,7 +571,7 @@
         <v>2.49</v>
       </c>
       <c r="E7" t="n">
-        <v>3.16</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="8">
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4.83</v>
+        <v>4.84</v>
       </c>
       <c r="C8" t="n">
         <v>4.19</v>
@@ -590,7 +590,7 @@
         <v>6.26</v>
       </c>
       <c r="E8" t="n">
-        <v>6.28</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="9">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5.89</v>
+        <v>5.83</v>
       </c>
       <c r="C9" t="n">
         <v>4.14</v>
@@ -609,7 +609,7 @@
         <v>6.3</v>
       </c>
       <c r="E9" t="n">
-        <v>5.65</v>
+        <v>5.67</v>
       </c>
     </row>
     <row r="10">
@@ -619,7 +619,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>14.7</v>
+        <v>14.84</v>
       </c>
       <c r="C10" t="n">
         <v>11.7</v>
@@ -628,7 +628,7 @@
         <v>15.98</v>
       </c>
       <c r="E10" t="n">
-        <v>14.05</v>
+        <v>14.02</v>
       </c>
     </row>
     <row r="11">
@@ -638,7 +638,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>22.09</v>
+        <v>22.18</v>
       </c>
       <c r="C11" t="n">
         <v>50.28</v>
@@ -647,7 +647,7 @@
         <v>19.47</v>
       </c>
       <c r="E11" t="n">
-        <v>25.44</v>
+        <v>25.41</v>
       </c>
     </row>
     <row r="12">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.72</v>
+        <v>2.65</v>
       </c>
       <c r="C12" t="n">
         <v>1.87</v>
@@ -666,7 +666,7 @@
         <v>2.38</v>
       </c>
       <c r="E12" t="n">
-        <v>2.18</v>
+        <v>2.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enforce notebook core logic boundary
</commit_message>
<xml_diff>
--- a/Symptom_Composition_Pivot_ChartReady.xlsx
+++ b/Symptom_Composition_Pivot_ChartReady.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,10 +451,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>other_hypercap_threshold</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>pco2_threshold_any</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>vbg_hypercap_threshold</t>
         </is>
@@ -473,9 +478,12 @@
         <v>3.13</v>
       </c>
       <c r="D2" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E2" t="n">
         <v>8.07</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>6.07</v>
       </c>
     </row>
@@ -492,9 +500,12 @@
         <v>4.34</v>
       </c>
       <c r="D3" t="n">
+        <v>7.56</v>
+      </c>
+      <c r="E3" t="n">
         <v>7.11</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>6.27</v>
       </c>
     </row>
@@ -505,16 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.77</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="C4" t="n">
         <v>5.04</v>
       </c>
       <c r="D4" t="n">
-        <v>7.78</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="E4" t="n">
-        <v>6.41</v>
+        <v>7.81</v>
+      </c>
+      <c r="F4" t="n">
+        <v>6.44</v>
       </c>
     </row>
     <row r="5">
@@ -530,9 +544,12 @@
         <v>6.91</v>
       </c>
       <c r="D5" t="n">
-        <v>10.13</v>
+        <v>10.33</v>
       </c>
       <c r="E5" t="n">
+        <v>10.12</v>
+      </c>
+      <c r="F5" t="n">
         <v>9.630000000000001</v>
       </c>
     </row>
@@ -549,10 +566,13 @@
         <v>6.71</v>
       </c>
       <c r="D6" t="n">
-        <v>14.04</v>
+        <v>13.49</v>
       </c>
       <c r="E6" t="n">
-        <v>14.89</v>
+        <v>14.03</v>
+      </c>
+      <c r="F6" t="n">
+        <v>14.88</v>
       </c>
     </row>
     <row r="7">
@@ -568,9 +588,12 @@
         <v>1.71</v>
       </c>
       <c r="D7" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="E7" t="n">
         <v>2.49</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>3.17</v>
       </c>
     </row>
@@ -587,9 +610,12 @@
         <v>4.19</v>
       </c>
       <c r="D8" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E8" t="n">
         <v>6.26</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>6.3</v>
       </c>
     </row>
@@ -606,10 +632,13 @@
         <v>4.14</v>
       </c>
       <c r="D9" t="n">
+        <v>6.27</v>
+      </c>
+      <c r="E9" t="n">
         <v>6.3</v>
       </c>
-      <c r="E9" t="n">
-        <v>5.67</v>
+      <c r="F9" t="n">
+        <v>5.66</v>
       </c>
     </row>
     <row r="10">
@@ -625,10 +654,13 @@
         <v>11.7</v>
       </c>
       <c r="D10" t="n">
-        <v>15.98</v>
+        <v>16.15</v>
       </c>
       <c r="E10" t="n">
-        <v>14.02</v>
+        <v>15.97</v>
+      </c>
+      <c r="F10" t="n">
+        <v>14.01</v>
       </c>
     </row>
     <row r="11">
@@ -644,10 +676,13 @@
         <v>50.28</v>
       </c>
       <c r="D11" t="n">
-        <v>19.47</v>
+        <v>18.84</v>
       </c>
       <c r="E11" t="n">
-        <v>25.41</v>
+        <v>19.46</v>
+      </c>
+      <c r="F11" t="n">
+        <v>25.4</v>
       </c>
     </row>
     <row r="12">
@@ -663,9 +698,12 @@
         <v>1.87</v>
       </c>
       <c r="D12" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="E12" t="n">
         <v>2.38</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>2.17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement blood gas contract plan
</commit_message>
<xml_diff>
--- a/Symptom_Composition_Pivot_ChartReady.xlsx
+++ b/Symptom_Composition_Pivot_ChartReady.xlsx
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.46</v>
+        <v>6.23</v>
       </c>
       <c r="C2" t="n">
-        <v>3.18</v>
+        <v>3.03</v>
       </c>
       <c r="D2" t="n">
-        <v>4.89</v>
+        <v>4.44</v>
       </c>
       <c r="E2" t="n">
-        <v>6.07</v>
+        <v>5.51</v>
       </c>
       <c r="F2" t="n">
-        <v>4.87</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.58</v>
+        <v>15.89</v>
       </c>
       <c r="C3" t="n">
-        <v>4.34</v>
+        <v>7.97</v>
       </c>
       <c r="D3" t="n">
-        <v>6.67</v>
+        <v>10.37</v>
       </c>
       <c r="E3" t="n">
-        <v>8.99</v>
+        <v>13.98</v>
       </c>
       <c r="F3" t="n">
-        <v>6.73</v>
+        <v>11.05</v>
       </c>
     </row>
     <row r="4">
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.88</v>
+        <v>6.38</v>
       </c>
       <c r="C4" t="n">
-        <v>5.4</v>
+        <v>5.7</v>
       </c>
       <c r="D4" t="n">
-        <v>7.48</v>
+        <v>7.7</v>
       </c>
       <c r="E4" t="n">
-        <v>6.42</v>
+        <v>6.56</v>
       </c>
       <c r="F4" t="n">
-        <v>5.78</v>
+        <v>6.55</v>
       </c>
     </row>
     <row r="5">
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.54</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>6.91</v>
+        <v>6.71</v>
       </c>
       <c r="D5" t="n">
-        <v>8.59</v>
+        <v>8.52</v>
       </c>
       <c r="E5" t="n">
-        <v>10.09</v>
+        <v>9.58</v>
       </c>
       <c r="F5" t="n">
-        <v>8.619999999999999</v>
+        <v>8.42</v>
       </c>
     </row>
     <row r="6">
@@ -560,19 +560,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11.83</v>
+        <v>12.08</v>
       </c>
       <c r="C6" t="n">
-        <v>6.71</v>
+        <v>7.21</v>
       </c>
       <c r="D6" t="n">
-        <v>11.7</v>
+        <v>12.07</v>
       </c>
       <c r="E6" t="n">
-        <v>11.83</v>
+        <v>12.15</v>
       </c>
       <c r="F6" t="n">
-        <v>10.94</v>
+        <v>11.42</v>
       </c>
     </row>
     <row r="7">
@@ -582,41 +582,41 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.72</v>
+        <v>4.15</v>
       </c>
       <c r="C7" t="n">
-        <v>4.44</v>
+        <v>4.14</v>
       </c>
       <c r="D7" t="n">
-        <v>5.48</v>
+        <v>5.19</v>
       </c>
       <c r="E7" t="n">
-        <v>5.01</v>
+        <v>4.61</v>
       </c>
       <c r="F7" t="n">
-        <v>5.16</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Symptom – Genitourinary</t>
+          <t>Symptom – Musculoskeletal</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.83</v>
+        <v>2.61</v>
       </c>
       <c r="C8" t="n">
-        <v>4.14</v>
+        <v>1.41</v>
       </c>
       <c r="D8" t="n">
-        <v>5.04</v>
+        <v>1.93</v>
       </c>
       <c r="E8" t="n">
-        <v>5.7</v>
+        <v>2.3</v>
       </c>
       <c r="F8" t="n">
-        <v>5.3</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="9">
@@ -626,19 +626,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>10.45</v>
+        <v>10.14</v>
       </c>
       <c r="C9" t="n">
-        <v>11.7</v>
+        <v>11.25</v>
       </c>
       <c r="D9" t="n">
-        <v>11.26</v>
+        <v>11.04</v>
       </c>
       <c r="E9" t="n">
-        <v>11.47</v>
+        <v>11.09</v>
       </c>
       <c r="F9" t="n">
-        <v>12.68</v>
+        <v>12.17</v>
       </c>
     </row>
     <row r="10">
@@ -648,19 +648,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>27.39</v>
+        <v>27.1</v>
       </c>
       <c r="C10" t="n">
-        <v>50.28</v>
+        <v>49.82</v>
       </c>
       <c r="D10" t="n">
-        <v>34.22</v>
+        <v>34.07</v>
       </c>
       <c r="E10" t="n">
-        <v>29.94</v>
+        <v>29.66</v>
       </c>
       <c r="F10" t="n">
-        <v>36.58</v>
+        <v>36.26</v>
       </c>
     </row>
     <row r="11">
@@ -670,19 +670,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.65</v>
+        <v>2.9</v>
       </c>
       <c r="C11" t="n">
-        <v>1.87</v>
+        <v>1.66</v>
       </c>
       <c r="D11" t="n">
-        <v>2.67</v>
+        <v>2.52</v>
       </c>
       <c r="E11" t="n">
-        <v>2.41</v>
+        <v>2.55</v>
       </c>
       <c r="F11" t="n">
-        <v>2.02</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="12">
@@ -692,16 +692,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.67</v>
+        <v>2.64</v>
       </c>
       <c r="C12" t="n">
-        <v>1.06</v>
+        <v>1.11</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>2.15</v>
       </c>
       <c r="E12" t="n">
-        <v>2.07</v>
+        <v>2.02</v>
       </c>
       <c r="F12" t="n">
         <v>1.33</v>

</xml_diff>